<commit_message>
Added code for fig 3
</commit_message>
<xml_diff>
--- a/figures/fig3.xlsx
+++ b/figures/fig3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joanna\Dropbox\Repositories\ISSP_Income-Pooling\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9288E16E-FD47-478C-91A9-8E8AB8F310EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FDC8E3-547C-410D-ACE5-170F97A3F5A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{153B74F1-F120-4CC5-9F95-BD6BE1F93E7B}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="9">
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="8">
   <si>
     <t>marst</t>
   </si>
@@ -65,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -98,7 +95,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -414,43 +411,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30171A97-052B-4150-9856-60C3CA9E6B55}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.06640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0.05</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>0.13621264</v>
@@ -464,16 +466,13 @@
       <c r="F2" s="2">
         <v>6.7127829999999999E-2</v>
       </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>0.05</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2">
         <v>0.10401515</v>
@@ -487,16 +486,13 @@
       <c r="F3" s="2">
         <v>0.21396432000000001</v>
       </c>
-      <c r="G3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <v>0.14543434</v>
@@ -510,16 +506,13 @@
       <c r="F4" s="2">
         <v>6.9914909999999997E-2</v>
       </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2">
         <v>0.11414272</v>
@@ -533,16 +526,13 @@
       <c r="F5" s="2">
         <v>0.21647293000000001</v>
       </c>
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>0.09</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2">
         <v>0.15508229000000001</v>
@@ -556,16 +546,13 @@
       <c r="F6" s="2">
         <v>7.2735750000000002E-2</v>
       </c>
-      <c r="G6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>0.09</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2">
         <v>0.12497453</v>
@@ -579,16 +566,13 @@
       <c r="F7" s="2">
         <v>0.21858141</v>
       </c>
-      <c r="G7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>0.11</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2">
         <v>0.16515367</v>
@@ -602,16 +586,13 @@
       <c r="F8" s="2">
         <v>7.5583020000000001E-2</v>
       </c>
-      <c r="G8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>0.11</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="2">
         <v>0.13652278000000001</v>
@@ -625,16 +606,13 @@
       <c r="F9" s="2">
         <v>0.2202711</v>
       </c>
-      <c r="G9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>0.13</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2">
         <v>0.17564307000000001</v>
@@ -648,16 +626,13 @@
       <c r="F10" s="2">
         <v>7.8448879999999999E-2</v>
       </c>
-      <c r="G10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>0.13</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" s="2">
         <v>0.14879528</v>
@@ -671,16 +646,13 @@
       <c r="F11" s="2">
         <v>0.22152595</v>
       </c>
-      <c r="G11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>0.15</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2">
         <v>0.18654240999999999</v>
@@ -694,16 +666,13 @@
       <c r="F12" s="2">
         <v>8.132499E-2</v>
       </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>0.15</v>
       </c>
       <c r="B13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="2">
         <v>0.16179515999999999</v>
@@ -717,16 +686,13 @@
       <c r="F13" s="2">
         <v>0.22233280999999999</v>
       </c>
-      <c r="G13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>0.17</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2">
         <v>0.19784086000000001</v>
@@ -740,16 +706,13 @@
       <c r="F14" s="2">
         <v>8.4202589999999994E-2</v>
       </c>
-      <c r="G14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>0.17</v>
       </c>
       <c r="B15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" s="2">
         <v>0.17552042000000001</v>
@@ -763,16 +726,13 @@
       <c r="F15" s="2">
         <v>0.22268162999999999</v>
       </c>
-      <c r="G15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>0.19</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2">
         <v>0.20952488999999999</v>
@@ -786,16 +746,13 @@
       <c r="F16" s="2">
         <v>8.7072549999999999E-2</v>
       </c>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>0.19</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="2">
         <v>0.18996378999999999</v>
@@ -809,16 +766,13 @@
       <c r="F17" s="2">
         <v>0.22256567999999999</v>
       </c>
-      <c r="G17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>0.21</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2">
         <v>0.22157822999999999</v>
@@ -832,16 +786,13 @@
       <c r="F18" s="2">
         <v>8.9925469999999993E-2</v>
       </c>
-      <c r="G18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>0.21</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="2">
         <v>0.20511245</v>
@@ -855,16 +806,13 @@
       <c r="F19" s="2">
         <v>0.22198166</v>
       </c>
-      <c r="G19" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>0.23</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2">
         <v>0.23398200999999999</v>
@@ -878,16 +826,13 @@
       <c r="F20" s="2">
         <v>9.2751730000000004E-2</v>
       </c>
-      <c r="G20" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>0.23</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" s="2">
         <v>0.22094801</v>
@@ -901,16 +846,13 @@
       <c r="F21" s="2">
         <v>0.22092978999999999</v>
       </c>
-      <c r="G21" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>0.25</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2">
         <v>0.24671483</v>
@@ -924,16 +866,13 @@
       <c r="F22" s="2">
         <v>9.5541580000000001E-2</v>
       </c>
-      <c r="G22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>0.25</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" s="2">
         <v>0.23744638000000001</v>
@@ -947,16 +886,13 @@
       <c r="F23" s="2">
         <v>0.21941385999999999</v>
       </c>
-      <c r="G23" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>0.27</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2">
         <v>0.25975294999999998</v>
@@ -970,16 +906,13 @@
       <c r="F24" s="2">
         <v>9.8285280000000003E-2</v>
       </c>
-      <c r="G24" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>0.27</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" s="2">
         <v>0.25457794</v>
@@ -993,16 +926,13 @@
       <c r="F25" s="2">
         <v>0.21744124000000001</v>
       </c>
-      <c r="G25" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>0.28999999999999998</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="2">
         <v>0.27307048</v>
@@ -1016,16 +946,13 @@
       <c r="F26" s="2">
         <v>0.10097312</v>
       </c>
-      <c r="G26" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>0.28999999999999998</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" s="2">
         <v>0.27230759999999998</v>
@@ -1039,16 +966,13 @@
       <c r="F27" s="2">
         <v>0.21502278999999999</v>
       </c>
-      <c r="G27" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>0.31</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2">
         <v>0.28663967000000001</v>
@@ -1062,16 +986,13 @@
       <c r="F28" s="2">
         <v>0.10359556</v>
       </c>
-      <c r="G28" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>0.31</v>
       </c>
       <c r="B29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="2">
         <v>0.29059519</v>
@@ -1085,16 +1006,13 @@
       <c r="F29" s="2">
         <v>0.21217273</v>
       </c>
-      <c r="G29" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>0.33</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" s="2">
         <v>0.30043112</v>
@@ -1108,16 +1026,13 @@
       <c r="F30" s="2">
         <v>0.10614334</v>
       </c>
-      <c r="G30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>0.33</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31" s="2">
         <v>0.30939559</v>
@@ -1131,16 +1046,13 @@
       <c r="F31" s="2">
         <v>0.20890849</v>
       </c>
-      <c r="G31" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>0.35</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" s="2">
         <v>0.31441406999999999</v>
@@ -1154,16 +1066,13 @@
       <c r="F32" s="2">
         <v>0.10860752</v>
       </c>
-      <c r="G32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>0.35</v>
       </c>
       <c r="B33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C33" s="2">
         <v>0.32865928999999999</v>
@@ -1177,16 +1086,13 @@
       <c r="F33" s="2">
         <v>0.20525051</v>
       </c>
-      <c r="G33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>0.37</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" s="2">
         <v>0.32855684000000002</v>
@@ -1200,16 +1106,13 @@
       <c r="F34" s="2">
         <v>0.11097963</v>
       </c>
-      <c r="G34" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>0.37</v>
       </c>
       <c r="B35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" s="2">
         <v>0.34833286000000002</v>
@@ -1223,16 +1126,13 @@
       <c r="F35" s="2">
         <v>0.20122193999999999</v>
       </c>
-      <c r="G35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>0.39</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C36" s="2">
         <v>0.34282699</v>
@@ -1246,16 +1146,13 @@
       <c r="F36" s="2">
         <v>0.11325169</v>
       </c>
-      <c r="G36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>0.39</v>
       </c>
       <c r="B37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" s="2">
         <v>0.36835938000000001</v>
@@ -1269,16 +1166,13 @@
       <c r="F37" s="2">
         <v>0.19684839000000001</v>
       </c>
-      <c r="G37" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>0.41</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38" s="2">
         <v>0.35719186000000003</v>
@@ -1292,16 +1186,13 @@
       <c r="F38" s="2">
         <v>0.11541634000000001</v>
       </c>
-      <c r="G38" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>0.41</v>
       </c>
       <c r="B39" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39" s="2">
         <v>0.38867921999999999</v>
@@ -1315,16 +1206,13 @@
       <c r="F39" s="2">
         <v>0.19215757999999999</v>
       </c>
-      <c r="G39" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>0.43</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" s="2">
         <v>0.37161867999999998</v>
@@ -1338,16 +1226,13 @@
       <c r="F40" s="2">
         <v>0.11746687</v>
       </c>
-      <c r="G40" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>0.43</v>
       </c>
       <c r="B41" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="2">
         <v>0.40923046000000002</v>
@@ -1361,16 +1246,13 @@
       <c r="F41" s="2">
         <v>0.18717897999999999</v>
       </c>
-      <c r="G41" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>0.45</v>
       </c>
       <c r="B42" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" s="2">
         <v>0.38607507000000002</v>
@@ -1384,16 +1266,13 @@
       <c r="F42" s="2">
         <v>0.11939729</v>
       </c>
-      <c r="G42" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>0.45</v>
       </c>
       <c r="B43" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C43" s="2">
         <v>0.42994967000000001</v>
@@ -1407,16 +1286,13 @@
       <c r="F43" s="2">
         <v>0.18194350000000001</v>
       </c>
-      <c r="G43" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>0.47</v>
       </c>
       <c r="B44" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" s="2">
         <v>0.40052932000000002</v>
@@ -1430,16 +1306,13 @@
       <c r="F44" s="2">
         <v>0.12120234000000001</v>
       </c>
-      <c r="G44" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>0.47</v>
       </c>
       <c r="B45" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C45" s="2">
         <v>0.45077266999999999</v>
@@ -1453,16 +1326,13 @@
       <c r="F45" s="2">
         <v>0.17648301999999999</v>
       </c>
-      <c r="G45" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>0.49</v>
       </c>
       <c r="B46" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="2">
         <v>0.41495061</v>
@@ -1476,16 +1346,13 @@
       <c r="F46" s="2">
         <v>0.12287758999999999</v>
       </c>
-      <c r="G46" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>0.49</v>
       </c>
       <c r="B47" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C47" s="2">
         <v>0.47163500000000003</v>
@@ -1499,16 +1366,13 @@
       <c r="F47" s="2">
         <v>0.17083010000000001</v>
       </c>
-      <c r="G47" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>0.51</v>
       </c>
       <c r="B48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" s="2">
         <v>0.4293093</v>
@@ -1522,16 +1386,13 @@
       <c r="F48" s="2">
         <v>0.12441936000000001</v>
       </c>
-      <c r="G48" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>0.51</v>
       </c>
       <c r="B49" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" s="2">
         <v>0.49247268999999999</v>
@@ -1545,16 +1406,13 @@
       <c r="F49" s="2">
         <v>0.16501758999999999</v>
       </c>
-      <c r="G49" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>0.53</v>
       </c>
       <c r="B50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" s="2">
         <v>0.44357722999999999</v>
@@ -1568,16 +1426,13 @@
       <c r="F50" s="2">
         <v>0.12582483999999999</v>
       </c>
-      <c r="G50" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>0.53</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C51" s="2">
         <v>0.51322298</v>
@@ -1591,16 +1446,13 @@
       <c r="F51" s="2">
         <v>0.15907821999999999</v>
       </c>
-      <c r="G51" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>0.55000000000000004</v>
       </c>
       <c r="B52" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" s="2">
         <v>0.45772789000000003</v>
@@ -1614,16 +1466,13 @@
       <c r="F52" s="2">
         <v>0.12709200000000001</v>
       </c>
-      <c r="G52" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>0.55000000000000004</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C53" s="2">
         <v>0.53382485999999996</v>
@@ -1637,16 +1486,13 @@
       <c r="F53" s="2">
         <v>0.15304428</v>
       </c>
-      <c r="G53" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>0.56999999999999995</v>
       </c>
       <c r="B54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54" s="2">
         <v>0.4717364</v>
@@ -1660,16 +1506,13 @@
       <c r="F54" s="2">
         <v>0.12821958999999999</v>
       </c>
-      <c r="G54" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>0.56999999999999995</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55" s="2">
         <v>0.55421942999999996</v>
@@ -1683,16 +1526,13 @@
       <c r="F55" s="2">
         <v>0.14694736</v>
       </c>
-      <c r="G55" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>0.59</v>
       </c>
       <c r="B56" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" s="2">
         <v>0.48557995999999998</v>
@@ -1706,16 +1546,13 @@
       <c r="F56" s="2">
         <v>0.12920715999999999</v>
       </c>
-      <c r="G56" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>0.59</v>
       </c>
       <c r="B57" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C57" s="2">
         <v>0.57435082000000004</v>
@@ -1729,16 +1566,13 @@
       <c r="F57" s="2">
         <v>0.14081795</v>
       </c>
-      <c r="G57" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>0.61</v>
       </c>
       <c r="B58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C58" s="2">
         <v>0.49923773999999999</v>
@@ -1752,16 +1586,13 @@
       <c r="F58" s="2">
         <v>0.13005496999999999</v>
       </c>
-      <c r="G58" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>0.61</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C59" s="2">
         <v>0.59416639999999998</v>
@@ -1777,8 +1608,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:H174">
-    <sortCondition ref="H2:H174"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:G174">
+    <sortCondition ref="G2:G174"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>